<commit_message>
- Added answer.py - Change DB
</commit_message>
<xml_diff>
--- a/par_cls.xlsx
+++ b/par_cls.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="241">
   <si>
     <t xml:space="preserve">ДХ</t>
   </si>
@@ -181,6 +181,12 @@
     <t xml:space="preserve">йтеся</t>
   </si>
   <si>
+    <t xml:space="preserve">ДД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тися</t>
+  </si>
+  <si>
     <t xml:space="preserve">ПЯ</t>
   </si>
   <si>
@@ -728,6 +734,15 @@
   </si>
   <si>
     <t xml:space="preserve">М.в.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОР</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ОА</t>
   </si>
 </sst>
 </file>
@@ -825,17 +840,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D103" activeCellId="0" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.37651821862348"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.0445344129555"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.37651821862348"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.87449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.6558704453441"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.87449392712551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,18 +1119,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,13 +1135,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,13 +1149,13 @@
         <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,13 +1163,13 @@
         <v>2</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,7 +1183,7 @@
         <v>65</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,13 +1191,13 @@
         <v>2</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,7 +1211,7 @@
         <v>70</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,7 +1225,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,13 +1233,13 @@
         <v>2</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="D28" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1235,13 +1247,13 @@
         <v>2</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="D29" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,13 +1261,13 @@
         <v>2</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,13 +1275,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,13 +1289,13 @@
         <v>2</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="D32" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,7 +1309,7 @@
         <v>89</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1311,7 +1323,7 @@
         <v>91</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,13 +1331,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="D35" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1339,7 +1351,7 @@
         <v>96</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,7 +1365,7 @@
         <v>98</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1367,7 +1379,7 @@
         <v>100</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,7 +1393,7 @@
         <v>102</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1395,7 +1407,7 @@
         <v>104</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1409,7 +1421,7 @@
         <v>106</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,13 +1429,13 @@
         <v>2</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="D42" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,13 +1443,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="D43" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,7 +1463,7 @@
         <v>114</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>110</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,7 +1477,7 @@
         <v>116</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1473,13 +1485,13 @@
         <v>2</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="D46" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,56 +1505,56 @@
         <v>121</v>
       </c>
       <c r="D47" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="C48" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="B49" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" s="0" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C52" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,13 +1562,13 @@
         <v>6</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="D53" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,13 +1576,13 @@
         <v>6</v>
       </c>
       <c r="B54" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="D54" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,13 +1590,13 @@
         <v>6</v>
       </c>
       <c r="B55" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="D55" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,7 +1610,7 @@
         <v>139</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1606,13 +1618,13 @@
         <v>6</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="D57" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1626,7 +1638,7 @@
         <v>144</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1634,13 +1646,13 @@
         <v>6</v>
       </c>
       <c r="B59" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C59" s="0" t="s">
-        <v>106</v>
-      </c>
       <c r="D59" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1648,13 +1660,13 @@
         <v>6</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,7 +1677,7 @@
         <v>149</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>150</v>
@@ -1682,7 +1694,7 @@
         <v>114</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,13 +1702,13 @@
         <v>6</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1704,10 +1716,10 @@
         <v>6</v>
       </c>
       <c r="B64" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>119</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>156</v>
@@ -1724,21 +1736,21 @@
         <v>121</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,7 +1761,7 @@
         <v>160</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>161</v>
@@ -1763,10 +1775,10 @@
         <v>162</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,13 +1786,13 @@
         <v>7</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>114</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,13 +1800,13 @@
         <v>7</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,10 +1817,10 @@
         <v>166</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,27 +1828,27 @@
         <v>7</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>121</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,13 +1856,13 @@
         <v>8</v>
       </c>
       <c r="B74" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="D74" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,13 +1870,13 @@
         <v>8</v>
       </c>
       <c r="B75" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="D75" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,13 +1884,13 @@
         <v>8</v>
       </c>
       <c r="B76" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C76" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="D76" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,13 +1898,13 @@
         <v>8</v>
       </c>
       <c r="B77" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C77" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="D77" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,13 +1912,13 @@
         <v>8</v>
       </c>
       <c r="B78" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="D78" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,13 +1926,13 @@
         <v>8</v>
       </c>
       <c r="B79" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C79" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="D79" s="0" t="s">
         <v>187</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1928,10 +1940,10 @@
         <v>8</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C80" s="0" t="s">
         <v>189</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>190</v>
@@ -1945,7 +1957,7 @@
         <v>191</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>192</v>
@@ -1959,10 +1971,10 @@
         <v>193</v>
       </c>
       <c r="C82" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D82" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,13 +1982,13 @@
         <v>8</v>
       </c>
       <c r="B83" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C83" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="D83" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,7 +2002,7 @@
         <v>199</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1998,24 +2010,24 @@
         <v>8</v>
       </c>
       <c r="B85" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C85" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="D85" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B86" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>204</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>205</v>
@@ -2029,10 +2041,10 @@
         <v>206</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>73</v>
+        <v>207</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2040,13 +2052,13 @@
         <v>9</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>96</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2054,13 +2066,13 @@
         <v>9</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>98</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>205</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2068,13 +2080,13 @@
         <v>9</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>100</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2100,7 @@
         <v>102</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>82</v>
+        <v>212</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,38 +2108,41 @@
         <v>9</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>104</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>106</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2135,13 +2150,10 @@
         <v>9</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>216</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2155,7 +2167,7 @@
         <v>114</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>73</v>
+        <v>218</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2163,13 +2175,13 @@
         <v>9</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>116</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>219</v>
+        <v>75</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,7 +2192,7 @@
         <v>220</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>221</v>
@@ -2197,21 +2209,21 @@
         <v>121</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>73</v>
+        <v>223</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>224</v>
+        <v>123</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>159</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,7 +2237,7 @@
         <v>226</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>227</v>
+        <v>161</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,13 +2245,13 @@
         <v>10</v>
       </c>
       <c r="B102" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C102" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="C102" s="0" t="s">
+      <c r="D102" s="0" t="s">
         <v>229</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,7 +2265,7 @@
         <v>231</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,7 +2279,7 @@
         <v>233</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,7 +2293,48 @@
         <v>235</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>227</v>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>